<commit_message>
Added Careers Page, Our Team Page
</commit_message>
<xml_diff>
--- a/URLsWithDomains.xlsx
+++ b/URLsWithDomains.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Site Map Done" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">URLsWithDomains!$A$1:$A$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">URLsWithDomains!$A$1:$A$27</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>URL</t>
   </si>
@@ -27,12 +27,6 @@
   </si>
   <si>
     <t>about.html</t>
-  </si>
-  <si>
-    <t>our-team.html</t>
-  </si>
-  <si>
-    <t>careers.html</t>
   </si>
   <si>
     <t>about-solar.html</t>
@@ -923,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -938,127 +932,112 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1078,7 +1057,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>

<commit_message>
Added About Solar Page
</commit_message>
<xml_diff>
--- a/URLsWithDomains.xlsx
+++ b/URLsWithDomains.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14295" windowHeight="4620"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14295" windowHeight="4620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="URLsWithDomains" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>URL</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>our-team.html</t>
+  </si>
+  <si>
+    <t>careers.html</t>
   </si>
 </sst>
 </file>
@@ -239,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,6 +423,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -580,8 +592,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -919,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1047,11 +1060,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -1070,6 +1081,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed About Solar Page
</commit_message>
<xml_diff>
--- a/URLsWithDomains.xlsx
+++ b/URLsWithDomains.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14295" windowHeight="4620" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14295" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="URLsWithDomains" sheetId="1" r:id="rId1"/>
     <sheet name="Site Map Done" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">URLsWithDomains!$A$1:$A$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">URLsWithDomains!$A$1:$A$26</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>URL</t>
   </si>
@@ -245,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,12 +423,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -594,7 +588,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -930,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -945,111 +939,106 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1062,7 +1051,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
Modified Nav Bar and Footer
</commit_message>
<xml_diff>
--- a/URLsWithDomains.xlsx
+++ b/URLsWithDomains.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14295" windowHeight="4620"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14295" windowHeight="4620" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="URLsWithDomains" sheetId="1" r:id="rId1"/>
     <sheet name="Site Map Done" sheetId="2" r:id="rId2"/>
+    <sheet name="Done Complete" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">URLsWithDomains!$A$1:$A$10</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>URL</t>
   </si>
@@ -102,6 +103,39 @@
   </si>
   <si>
     <t>careers.html</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>about-solar</t>
+  </si>
+  <si>
+    <t>blog</t>
+  </si>
+  <si>
+    <t>blog-post</t>
+  </si>
+  <si>
+    <t>brochures-technical-info</t>
+  </si>
+  <si>
+    <t>careers</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>clients</t>
+  </si>
+  <si>
+    <t>coming-soon</t>
+  </si>
+  <si>
+    <t>commercial-government</t>
+  </si>
+  <si>
+    <t>compare-plans-offers</t>
   </si>
 </sst>
 </file>
@@ -933,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -997,7 +1031,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,4 +1129,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>